<commit_message>
started RNN & LSTM notebook
</commit_message>
<xml_diff>
--- a/materials/07-recommender-collaborative-filtering/collab_filter.xlsx
+++ b/materials/07-recommender-collaborative-filtering/collab_filter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/b294776/Desktop/Workspace/Training/rstudio-conf-2020/dl-keras-tf/materials/07-recommender-collaborative-filtering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34D45750-3FE0-6D4E-B3AC-33AB5D2B19B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11735F7-0B4C-5849-9546-D4F321104670}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="1820" windowWidth="34660" windowHeight="24380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39700" yWindow="880" windowWidth="34660" windowHeight="24380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dotprod" sheetId="1" r:id="rId1"/>
@@ -2332,6 +2332,113 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFA81E8E-3376-4137-B126-61D3F5656D3A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B3:B18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="16">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="15">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <formats count="3">
+    <format dxfId="14">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="13">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="12">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4B556251-D0A3-4290-A5D7-C5203D1B35B6}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B21:B36" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
@@ -2431,123 +2538,16 @@
     <i/>
   </colItems>
   <formats count="3">
-    <format dxfId="14">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="13">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="12">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFA81E8E-3376-4137-B126-61D3F5656D3A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B3:B18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="16">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="15">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <formats count="3">
     <format dxfId="17">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
     <format dxfId="16">
-      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
     <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
-          <reference field="0" count="0"/>
+          <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
@@ -3199,7 +3199,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:V41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
@@ -60490,7 +60490,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>